<commit_message>
update diary and backlog
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7081.s2013.black/doc/taskRepository/CS1/Task10/scrum_ProductSprintBacklog_Black.xlsx
+++ b/ch.bfh.bti7081.s2013.black/doc/taskRepository/CS1/Task10/scrum_ProductSprintBacklog_Black.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Inversini\Desktop\BFH\develop\SEngineering\ch.bfh.bti7081.s2013.black\ch.bfh.bti7081.s2013.black\doc\taskRepository\CS1\Task10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11535" activeTab="2"/>
+    <workbookView xWindow="900" yWindow="160" windowWidth="28100" windowHeight="15740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,12 +15,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint1 Backlog'!$A$1:$K$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint2 Backlog'!$A$1:$K$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -463,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -498,7 +498,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -713,18 +713,18 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="28">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="56">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -776,7 +776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="42">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -802,7 +802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="70">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -828,7 +828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="42">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -854,14 +854,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" s="12" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -871,22 +876,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -921,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="14">
         <v>2.1</v>
       </c>
@@ -956,7 +961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="14">
         <v>2.2000000000000002</v>
       </c>
@@ -991,7 +996,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="14">
         <v>2.2999999999999998</v>
       </c>
@@ -1026,7 +1031,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="14">
         <v>2.4</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="14">
         <v>2.5</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="14">
         <v>2.6</v>
       </c>
@@ -1131,7 +1136,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="14">
         <v>2.7</v>
       </c>
@@ -1166,7 +1171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="14">
         <v>2.8</v>
       </c>
@@ -1201,7 +1206,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="15">
         <v>2.9</v>
       </c>
@@ -1236,10 +1241,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="15"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="15"/>
     </row>
   </sheetData>
@@ -1248,34 +1253,39 @@
     <sortCondition ref="B2:B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="15" t="s">
         <v>71</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28">
       <c r="A3" s="14">
         <v>2.11</v>
       </c>
@@ -1368,7 +1378,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="14">
         <v>2.12</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="15" t="s">
         <v>74</v>
       </c>
@@ -1426,7 +1436,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="14" t="s">
         <v>80</v>
       </c>
@@ -1455,7 +1465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="14" t="s">
         <v>84</v>
       </c>
@@ -1484,7 +1494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="14" t="s">
         <v>87</v>
       </c>
@@ -1513,7 +1523,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="28">
       <c r="A9" s="14" t="s">
         <v>90</v>
       </c>
@@ -1538,11 +1548,17 @@
       <c r="H9" t="s">
         <v>56</v>
       </c>
+      <c r="I9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
       <c r="K9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="14" t="s">
         <v>94</v>
       </c>
@@ -1568,11 +1584,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:K5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
daily scrum, sprint review, sprint planing sprint 3
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7081.s2013.black/doc/taskRepository/CS1/Task10/scrum_ProductSprintBacklog_Black.xlsx
+++ b/ch.bfh.bti7081.s2013.black/doc/taskRepository/CS1/Task10/scrum_ProductSprintBacklog_Black.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="900" yWindow="150" windowWidth="28110" windowHeight="12810" activeTab="3"/>
+    <workbookView xWindow="900" yWindow="150" windowWidth="28110" windowHeight="12810" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint1 Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint2 Backlog" sheetId="4" r:id="rId3"/>
     <sheet name="Sprint3 Backlog" sheetId="5" r:id="rId4"/>
+    <sheet name="Sprint4 Backlog" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint1 Backlog'!$A$1:$K$14</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -322,6 +323,69 @@
   </si>
   <si>
     <t>2.11</t>
+  </si>
+  <si>
+    <t>2.12</t>
+  </si>
+  <si>
+    <t>2.19</t>
+  </si>
+  <si>
+    <t>Clienthistory erfassen</t>
+  </si>
+  <si>
+    <t>GUI, DB, Businesslogic</t>
+  </si>
+  <si>
+    <t>in work</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>Test erfassen für 2.19</t>
+  </si>
+  <si>
+    <t>Tests schreiben für ein TDD für Punkt 2.19</t>
+  </si>
+  <si>
+    <t>2.21</t>
+  </si>
+  <si>
+    <t>Junit testing</t>
+  </si>
+  <si>
+    <t>Code analysieren mit Junit test</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Daniel, Michael</t>
+  </si>
+  <si>
+    <t>2.22</t>
+  </si>
+  <si>
+    <t>Code analysis</t>
+  </si>
+  <si>
+    <t>Code analysieren mit Google CodePro Analytix</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>2.23</t>
+  </si>
+  <si>
+    <t>History zu Clienten hinzufügen (DB)</t>
+  </si>
+  <si>
+    <t>History zu Clienten hinzufügen (GUI)</t>
+  </si>
+  <si>
+    <t>DB, Businesslogic</t>
   </si>
 </sst>
 </file>
@@ -377,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -413,6 +477,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -719,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1650,7 +1715,244 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,7 +2017,7 @@
         <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
         <v>56</v>
@@ -1725,8 +2027,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>2.12</v>
+      <c r="A3" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="B3">
         <v>3</v>

</xml_diff>

<commit_message>
updated sprint backlog & tests
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7081.s2013.black/doc/taskRepository/CS1/Task10/scrum_ProductSprintBacklog_Black.xlsx
+++ b/ch.bfh.bti7081.s2013.black/doc/taskRepository/CS1/Task10/scrum_ProductSprintBacklog_Black.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Inversini\Desktop\BFH\develop\SEngineering\ch.bfh.bti7081.s2013.black\ch.bfh.bti7081.s2013.black\doc\taskRepository\CS1\Task10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="900" yWindow="156" windowWidth="23256" windowHeight="12816" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="900" yWindow="150" windowWidth="23250" windowHeight="12810" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -533,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -783,15 +788,15 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -820,7 +825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -846,7 +851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -872,7 +877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -898,7 +903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -924,7 +929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>95</v>
       </c>
@@ -946,22 +951,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="14" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -996,7 +1001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>2.1</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2.2000000000000002</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>2.2999999999999998</v>
       </c>
@@ -1101,7 +1106,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>2.4</v>
       </c>
@@ -1136,7 +1141,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>2.5</v>
       </c>
@@ -1171,7 +1176,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>2.6</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>2.7</v>
       </c>
@@ -1241,7 +1246,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>2.8</v>
       </c>
@@ -1276,7 +1281,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>2.9</v>
       </c>
@@ -1311,10 +1316,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
     </row>
   </sheetData>
@@ -1340,22 +1345,22 @@
       <selection activeCell="G19" sqref="G18:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="14" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1430,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2.11</v>
       </c>
@@ -1454,7 +1459,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>2.12</v>
       </c>
@@ -1483,7 +1488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>73</v>
       </c>
@@ -1518,7 +1523,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -1553,7 +1558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>82</v>
       </c>
@@ -1588,7 +1593,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>85</v>
       </c>
@@ -1623,7 +1628,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>88</v>
       </c>
@@ -1658,7 +1663,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>92</v>
       </c>
@@ -1713,15 +1718,15 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1756,7 +1761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>98</v>
       </c>
@@ -1782,13 +1787,13 @@
         <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>102</v>
       </c>
@@ -1820,10 +1825,10 @@
         <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>105</v>
       </c>
@@ -1849,13 +1854,13 @@
         <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>110</v>
       </c>
@@ -1880,11 +1885,14 @@
       <c r="H5" t="s">
         <v>43</v>
       </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
       <c r="K5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>114</v>
       </c>
@@ -1913,40 +1921,40 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
     </row>
-    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
     </row>
   </sheetData>
@@ -1962,14 +1970,14 @@
       <selection activeCell="A2" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +2012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>96</v>
       </c>
@@ -2033,7 +2041,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>97</v>
       </c>
@@ -2062,49 +2070,49 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
     </row>
-    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
     </row>
   </sheetData>

</xml_diff>